<commit_message>
imported advertising and sales datasets
</commit_message>
<xml_diff>
--- a/data/advertising_cost.xlsx
+++ b/data/advertising_cost.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -132,12 +136,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="#,##0.##"/>
-    <numFmt numFmtId="178" formatCode="#,##0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.##"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -156,16 +163,28 @@
       <family val="2"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -180,79 +199,59 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-      <protection/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-      <protection/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-      <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0"/>
-    <cellStyle name="Percent" xfId="15"/>
-    <cellStyle name="Currency" xfId="16"/>
-    <cellStyle name="Currency [0]" xfId="17"/>
-    <cellStyle name="Comma" xfId="18"/>
-    <cellStyle name="Comma [0]" xfId="19"/>
+  <cellStyles count="8">
+    <cellStyle name="Comma" xfId="4"/>
+    <cellStyle name="Comma [0]" xfId="5"/>
+    <cellStyle name="Currency" xfId="2"/>
+    <cellStyle name="Currency [0]" xfId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -643,38 +642,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="25.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="70.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="12.75">
+    <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" ht="12.75">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="12.75">
+    <row r="5" spans="2:3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" ht="12.75">
+    <row r="8" spans="2:3">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="12.75">
+    <row r="10" spans="2:3">
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
@@ -682,7 +681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="12.75">
+    <row r="11" spans="2:3">
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
@@ -690,7 +689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="12.75">
+    <row r="12" spans="2:3">
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -698,7 +697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="12.75">
+    <row r="13" spans="2:3">
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
@@ -706,7 +705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="12.75">
+    <row r="14" spans="2:3">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -714,7 +713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="12.75">
+    <row r="15" spans="2:3">
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
@@ -722,7 +721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="12.75">
+    <row r="16" spans="2:3">
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -730,7 +729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="12.75">
+    <row r="17" spans="2:3">
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
@@ -738,7 +737,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="12.75">
+    <row r="18" spans="2:3">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
@@ -746,12 +745,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" ht="12.75">
+    <row r="20" spans="2:3">
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="12.75">
+    <row r="22" spans="2:3">
       <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
@@ -759,7 +758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="12.75">
+    <row r="23" spans="2:3">
       <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
@@ -767,7 +766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="12.75">
+    <row r="24" spans="2:3">
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -775,7 +774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="12.75">
+    <row r="25" spans="2:3">
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
@@ -786,41 +785,46 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" location="Data!A1" display="Access data"/>
-    <hyperlink ref="C25" r:id="rId1" display="639356"/>
+    <hyperlink ref="C25" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="B3:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="100.714285714286" customWidth="1"/>
-    <col min="3" max="3" width="27.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="12.75">
+    <row r="3" spans="2:3">
       <c r="B3" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" ht="12.75">
-      <c r="B4" s="5" t="s">
+    <row r="5" spans="2:3">
+      <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" ht="12.75">
       <c r="C5" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="12.75">
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
@@ -828,7 +832,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="12.75">
+    <row r="7" spans="2:3">
       <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
@@ -836,7 +840,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="12.75">
+    <row r="8" spans="2:3">
       <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
@@ -844,7 +848,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="12.75">
+    <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
@@ -852,7 +856,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="12.75">
+    <row r="10" spans="2:3">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -860,7 +864,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="12.75">
+    <row r="11" spans="2:3">
       <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
@@ -868,15 +872,15 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="12.75">
+    <row r="12" spans="2:3">
       <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="10">
-        <v>103.09999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="12.75">
+        <v>103.1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
       <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
@@ -884,7 +888,7 @@
         <v>102.7</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="12.75">
+    <row r="14" spans="2:3">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
@@ -892,7 +896,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="12.75">
+    <row r="15" spans="2:3">
       <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
@@ -903,5 +907,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>